<commit_message>
Commit Eleven - PDF robot
</commit_message>
<xml_diff>
--- a/Bot4/Robot4/realestatedata.xlsx
+++ b/Bot4/Robot4/realestatedata.xlsx
@@ -14,38 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
-  <si>
-    <t>Bulwer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Musgrave</t>
   </si>
   <si>
-    <t>R 2 350 000</t>
-  </si>
-  <si>
-    <t>151 m²</t>
-  </si>
-  <si>
-    <t>Point Waterfront</t>
-  </si>
-  <si>
     <t>Essenwood</t>
   </si>
   <si>
     <t>R 550 000</t>
   </si>
   <si>
-    <t>50 m²</t>
-  </si>
-  <si>
-    <t>R 800 000</t>
-  </si>
-  <si>
-    <t>61 m²</t>
-  </si>
-  <si>
     <t>R 895 000</t>
   </si>
   <si>
@@ -91,70 +70,103 @@
     <t>Location</t>
   </si>
   <si>
-    <t>R 1 195 000</t>
-  </si>
-  <si>
-    <t>812 m²</t>
-  </si>
-  <si>
-    <t>Carrington Heights</t>
-  </si>
-  <si>
-    <t>Reservoir Hills</t>
-  </si>
-  <si>
-    <t>R 1 295 000</t>
-  </si>
-  <si>
-    <t>689 m²</t>
-  </si>
-  <si>
     <t>R 1 495 000</t>
   </si>
   <si>
-    <t>1 173 m²</t>
-  </si>
-  <si>
-    <t>R 1 750 000</t>
-  </si>
-  <si>
-    <t>929 m²</t>
-  </si>
-  <si>
-    <t>Mount Vernon</t>
-  </si>
-  <si>
-    <t>Bluff</t>
-  </si>
-  <si>
-    <t>R 2 395 000</t>
-  </si>
-  <si>
-    <t>1 744 m²</t>
-  </si>
-  <si>
-    <t>R 2 500 000</t>
-  </si>
-  <si>
-    <t>932 m²</t>
-  </si>
-  <si>
-    <t>Brighton Beach</t>
-  </si>
-  <si>
-    <t>R 3 070 000</t>
-  </si>
-  <si>
-    <t>156 m²</t>
-  </si>
-  <si>
-    <t>R 495 000</t>
-  </si>
-  <si>
-    <t>600 m²</t>
-  </si>
-  <si>
-    <t>Inanda</t>
+    <t>R 1 300 000</t>
+  </si>
+  <si>
+    <t>74 m²</t>
+  </si>
+  <si>
+    <t>Sherwood</t>
+  </si>
+  <si>
+    <t>R 1 350 000</t>
+  </si>
+  <si>
+    <t>111 m²</t>
+  </si>
+  <si>
+    <t>90 m²</t>
+  </si>
+  <si>
+    <t>North Beach</t>
+  </si>
+  <si>
+    <t>R 1 500 000</t>
+  </si>
+  <si>
+    <t>77 m²</t>
+  </si>
+  <si>
+    <t>R 1 690 000</t>
+  </si>
+  <si>
+    <t>146 m²</t>
+  </si>
+  <si>
+    <t>R 1 700 000</t>
+  </si>
+  <si>
+    <t>164 m²</t>
+  </si>
+  <si>
+    <t>Glenwood</t>
+  </si>
+  <si>
+    <t>R 2 200 000</t>
+  </si>
+  <si>
+    <t>210 m²</t>
+  </si>
+  <si>
+    <t>South Beach</t>
+  </si>
+  <si>
+    <t>R 2 325 000</t>
+  </si>
+  <si>
+    <t>296 m²</t>
+  </si>
+  <si>
+    <t>R 3 395 000</t>
+  </si>
+  <si>
+    <t>209 m²</t>
+  </si>
+  <si>
+    <t>R 499 000</t>
+  </si>
+  <si>
+    <t>73 m²</t>
+  </si>
+  <si>
+    <t>Umbilo</t>
+  </si>
+  <si>
+    <t>51 m²</t>
+  </si>
+  <si>
+    <t>Esplanade</t>
+  </si>
+  <si>
+    <t>R 595 000</t>
+  </si>
+  <si>
+    <t>46 m²</t>
+  </si>
+  <si>
+    <t>R 650 000</t>
+  </si>
+  <si>
+    <t>81 m²</t>
+  </si>
+  <si>
+    <t>R 725 000</t>
+  </si>
+  <si>
+    <t>565 m²</t>
   </si>
 </sst>
 </file>
@@ -501,194 +513,194 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -697,100 +709,100 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B14">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -799,15 +811,15 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>2.5</v>
@@ -816,15 +828,15 @@
         <v>1.5</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -833,15 +845,15 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -850,10 +862,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>